<commit_message>
update BOM and Impl Chart
</commit_message>
<xml_diff>
--- a/docs/FeatherWing_Implementation_Chart.xlsx
+++ b/docs/FeatherWing_Implementation_Chart.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\GitHub\AD9833_FeatherWing\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1E9229-776D-42D4-8EE7-523BFF3820DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023EFB02-CD78-4F70-A757-BE32DC878322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="-15870" windowWidth="25440" windowHeight="15990" xr2:uid="{C7EDD24A-D5F0-40E7-9C67-C76A930CACB0}"/>
+    <workbookView xWindow="3360" yWindow="-14670" windowWidth="21645" windowHeight="14340" xr2:uid="{C7EDD24A-D5F0-40E7-9C67-C76A930CACB0}"/>
   </bookViews>
   <sheets>
     <sheet name="FeatherWing Impl Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>FeatherWing Implementation Chart</t>
   </si>

</xml_diff>